<commit_message>
feat: add opção para escolher o tipo de variável a ser analisada
</commit_message>
<xml_diff>
--- a/resultados_variavel_xm.xlsx
+++ b/resultados_variavel_xm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,13 +452,35 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-406.6570854713468</v>
+        <v>320.4131556305247</v>
       </c>
       <c r="B2" t="n">
-        <v>2766.55</v>
+        <v>3289.743</v>
       </c>
       <c r="C2" t="n">
-        <v>-680.287</v>
+        <v>-775.769</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>441.6047391640358</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3289.743</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-775.769</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>431.9462277151515</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3289.743</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-775.769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>